<commit_message>
Update CMU_CS 246 BIS_TEAM2_TEST CASE(version 2.0).xlsx
</commit_message>
<xml_diff>
--- a/3. Software Configuration Management Part 1/2. Group/CMU_CS 246 BIS_TEAM2_TEST CASE(version 2.0).xlsx
+++ b/3. Software Configuration Management Part 1/2. Group/CMU_CS 246 BIS_TEAM2_TEST CASE(version 2.0).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Application Dev\CMU_CS-246-BIS_TEAM2\3. Software Configuration Management Part 1\2. Group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS\Documents\GitHub\CMU_CS-246-BIS_TEAM2\3. Software Configuration Management Part 1\2. Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47FDC73-E1F0-46C9-9F3E-0E683652C596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5A6A00-F751-4696-93D0-B1E926437BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1056,7 +1056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1172,46 +1172,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1224,12 +1184,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1251,6 +1205,49 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3860,14 +3857,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="59"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -4069,7 +4066,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="60" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -4100,7 +4097,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="47"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
@@ -4129,7 +4126,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
@@ -4158,7 +4155,7 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="47"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
@@ -4187,7 +4184,7 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
@@ -4243,7 +4240,7 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="60" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -4274,7 +4271,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
@@ -4303,7 +4300,7 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="47"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
@@ -4332,7 +4329,7 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
@@ -4452,19 +4449,19 @@
       <c r="Y20" s="9"/>
     </row>
     <row r="21" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="61">
+      <c r="A21" s="43">
         <v>1</v>
       </c>
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="62" t="s">
+      <c r="D21" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="63">
+      <c r="E21" s="45">
         <f t="shared" ref="E21:E25" si="0">DATE(2024,1,27)</f>
         <v>45318</v>
       </c>
@@ -4490,19 +4487,19 @@
       <c r="Y21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61">
+      <c r="A22" s="43">
         <v>2</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="63">
+      <c r="E22" s="45">
         <f t="shared" si="0"/>
         <v>45318</v>
       </c>
@@ -4528,19 +4525,19 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="61">
+      <c r="A23" s="43">
         <v>3</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="62" t="s">
+      <c r="D23" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="63">
+      <c r="E23" s="45">
         <f t="shared" si="0"/>
         <v>45318</v>
       </c>
@@ -4566,19 +4563,19 @@
       <c r="Y23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="61">
+      <c r="A24" s="43">
         <v>4</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="C24" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="62" t="s">
+      <c r="D24" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="63">
+      <c r="E24" s="45">
         <f t="shared" si="0"/>
         <v>45318</v>
       </c>
@@ -4604,19 +4601,19 @@
       <c r="Y24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="61">
+      <c r="A25" s="43">
         <v>5</v>
       </c>
-      <c r="B25" s="61" t="s">
+      <c r="B25" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="63">
+      <c r="E25" s="45">
         <f t="shared" si="0"/>
         <v>45318</v>
       </c>
@@ -4642,19 +4639,19 @@
       <c r="Y25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="61">
+      <c r="A26" s="43">
         <v>6</v>
       </c>
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="49" t="s">
         <v>164</v>
       </c>
-      <c r="C26" s="65" t="s">
+      <c r="C26" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="D26" s="65" t="s">
+      <c r="D26" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="63">
+      <c r="E26" s="45">
         <v>45354</v>
       </c>
       <c r="F26" s="1"/>
@@ -4679,19 +4676,19 @@
       <c r="Y26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="61">
+      <c r="A27" s="43">
         <v>7</v>
       </c>
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="D27" s="66" t="s">
+      <c r="D27" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="E27" s="63">
+      <c r="E27" s="45">
         <v>45354</v>
       </c>
       <c r="F27" s="1"/>
@@ -4716,19 +4713,19 @@
       <c r="Y27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="61">
+      <c r="A28" s="43">
         <v>8</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="E28" s="63">
+      <c r="E28" s="45">
         <v>45354</v>
       </c>
       <c r="F28" s="1"/>
@@ -4753,19 +4750,19 @@
       <c r="Y28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="61">
+      <c r="A29" s="43">
         <v>9</v>
       </c>
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="49" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="D29" s="66" t="s">
+      <c r="D29" s="48" t="s">
         <v>161</v>
       </c>
-      <c r="E29" s="63">
+      <c r="E29" s="45">
         <v>45354</v>
       </c>
       <c r="F29" s="1"/>
@@ -4790,19 +4787,19 @@
       <c r="Y29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="61">
+      <c r="A30" s="43">
         <v>10</v>
       </c>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="D30" s="66" t="s">
+      <c r="D30" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="E30" s="63">
+      <c r="E30" s="45">
         <v>45354</v>
       </c>
       <c r="F30" s="1"/>
@@ -4827,7 +4824,7 @@
       <c r="Y30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="60"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -11273,7 +11270,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="C12" sqref="C12:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11294,14 +11291,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="68" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -11312,14 +11309,14 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -11330,12 +11327,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -11346,28 +11343,28 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="68" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="31"/>
-      <c r="H4" s="76"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -11390,8 +11387,8 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>2</v>
       </c>
@@ -11414,10 +11411,10 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -11440,8 +11437,8 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>2</v>
       </c>
@@ -11478,60 +11475,60 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -11541,22 +11538,22 @@
         <f>CONCATENATE($C$2, " - ", A12)</f>
         <v>BS - 1</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="F12" s="74" t="s">
+      <c r="F12" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="G12" s="75" t="s">
+      <c r="G12" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="H12" s="74" t="s">
+      <c r="H12" s="54" t="s">
         <v>203</v>
       </c>
       <c r="I12" s="11">
@@ -11571,7 +11568,7 @@
       <c r="L12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="73" t="s">
+      <c r="M12" s="53" t="s">
         <v>13</v>
       </c>
     </row>
@@ -11583,22 +11580,22 @@
         <f t="shared" ref="B13" si="0">CONCATENATE($C$2, " - ", A13)</f>
         <v>BS - 2</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="E13" s="70" t="s">
+      <c r="E13" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="F13" s="74" t="s">
+      <c r="F13" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="G13" s="72" t="s">
+      <c r="G13" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="H13" s="74" t="s">
+      <c r="H13" s="54" t="s">
         <v>200</v>
       </c>
       <c r="I13" s="11">
@@ -11613,12 +11610,26 @@
       <c r="L13" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="73" t="s">
+      <c r="M13" s="53" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
@@ -11628,20 +11639,6 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J13 L13">
     <cfRule type="containsText" dxfId="31" priority="9" operator="containsText" text="FAIL">
@@ -11757,8 +11754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79380B9-BFC8-4681-924C-8CE0F0A758F3}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11771,7 +11768,7 @@
     <col min="6" max="6" width="20.796875" customWidth="1"/>
     <col min="7" max="7" width="14.59765625" customWidth="1"/>
     <col min="8" max="8" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
@@ -11779,14 +11776,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="68" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="74" t="s">
         <v>162</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -11797,14 +11794,14 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="75" t="s">
         <v>205</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -11815,12 +11812,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -11831,28 +11828,28 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="68" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="31"/>
-      <c r="H4" s="76"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -11875,8 +11872,8 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>2</v>
       </c>
@@ -11899,10 +11896,10 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -11925,8 +11922,8 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>2</v>
       </c>
@@ -11963,60 +11960,60 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="84" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -12026,16 +12023,16 @@
         <f>CONCATENATE($C$2, " - ", A12)</f>
         <v>CA - 1</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="F12" s="74" t="s">
+      <c r="F12" s="54" t="s">
         <v>86</v>
       </c>
       <c r="G12" s="42" t="s">
@@ -12056,7 +12053,7 @@
       <c r="L12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="73" t="s">
+      <c r="M12" s="53" t="s">
         <v>11</v>
       </c>
     </row>
@@ -12068,22 +12065,22 @@
         <f t="shared" ref="B13" si="0">CONCATENATE($C$2, " - ", A13)</f>
         <v>CA - 2</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="E13" s="70" t="s">
+      <c r="E13" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="F13" s="74" t="s">
+      <c r="F13" s="54" t="s">
         <v>206</v>
       </c>
-      <c r="G13" s="72" t="s">
+      <c r="G13" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="H13" s="74" t="s">
+      <c r="H13" s="54" t="s">
         <v>200</v>
       </c>
       <c r="I13" s="11">
@@ -12098,12 +12095,26 @@
       <c r="L13" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="73" t="s">
+      <c r="M13" s="53" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
@@ -12113,20 +12124,6 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J13 L13">
     <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="FAIL">
@@ -12265,14 +12262,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -12283,14 +12280,14 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -12301,12 +12298,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -12317,14 +12314,14 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="H4" s="13"/>
@@ -12334,10 +12331,10 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -12359,8 +12356,8 @@
       <c r="L5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>9</v>
       </c>
@@ -12385,10 +12382,10 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -12410,8 +12407,8 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>9</v>
       </c>
@@ -12450,60 +12447,60 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -13932,6 +13929,20 @@
     <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="E10:E11"/>
@@ -13941,20 +13952,6 @@
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J12:J17 J19:J20 L12:L17 L19:L20">
     <cfRule type="containsText" dxfId="215" priority="1" operator="containsText" text="FAIL">
@@ -14251,14 +14248,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -14270,14 +14267,14 @@
       <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -14289,12 +14286,12 @@
       <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -14306,14 +14303,14 @@
       <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="31"/>
@@ -14325,10 +14322,10 @@
       <c r="M4" s="31"/>
     </row>
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -14352,8 +14349,8 @@
       <c r="M5" s="31"/>
     </row>
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>10</v>
       </c>
@@ -14377,10 +14374,10 @@
       <c r="M6" s="31"/>
     </row>
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -14404,8 +14401,8 @@
       <c r="M7" s="31"/>
     </row>
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>10</v>
       </c>
@@ -14444,60 +14441,60 @@
       <c r="M9" s="31"/>
     </row>
     <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -15908,6 +15905,20 @@
     <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="E10:E11"/>
@@ -15917,20 +15928,6 @@
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J21 L21">
     <cfRule type="containsText" dxfId="167" priority="1" operator="containsText" text="FAIL">
@@ -16021,14 +16018,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -16039,14 +16036,14 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -16057,12 +16054,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -16073,14 +16070,14 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="H4" s="13"/>
@@ -16090,10 +16087,10 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -16115,8 +16112,8 @@
       <c r="L5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>9</v>
       </c>
@@ -16141,10 +16138,10 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -16166,8 +16163,8 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>9</v>
       </c>
@@ -16206,60 +16203,60 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -17688,6 +17685,20 @@
     <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="E10:E11"/>
@@ -17697,20 +17708,6 @@
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J12:J17 J19:J20 L12:L17 L19:L20">
     <cfRule type="containsText" dxfId="159" priority="1" operator="containsText" text="FAIL">
@@ -18007,14 +18004,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -18025,14 +18022,14 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -18043,12 +18040,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -18059,14 +18056,14 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="H4" s="13"/>
@@ -18076,10 +18073,10 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -18101,8 +18098,8 @@
       <c r="L5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>10</v>
       </c>
@@ -18127,10 +18124,10 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -18152,8 +18149,8 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>10</v>
       </c>
@@ -18192,60 +18189,60 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -19715,6 +19712,20 @@
     <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="E10:E11"/>
@@ -19724,20 +19735,6 @@
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J12:J17 J19:J21 L12:L17 L19:L21">
     <cfRule type="containsText" dxfId="111" priority="1" operator="containsText" text="SKIPPED">
@@ -19888,14 +19885,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="50" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -19907,14 +19904,14 @@
       <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -19926,12 +19923,12 @@
       <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -19943,14 +19940,14 @@
       <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="31"/>
@@ -19962,10 +19959,10 @@
       <c r="M4" s="31"/>
     </row>
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -19989,8 +19986,8 @@
       <c r="M5" s="31"/>
     </row>
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>12</v>
       </c>
@@ -20014,10 +20011,10 @@
       <c r="M6" s="31"/>
     </row>
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -20041,8 +20038,8 @@
       <c r="M7" s="31"/>
     </row>
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>12</v>
       </c>
@@ -20081,60 +20078,60 @@
       <c r="M9" s="31"/>
     </row>
     <row r="10" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="84" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -20317,7 +20314,7 @@
       <c r="E16" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="71" t="s">
+      <c r="F16" s="51" t="s">
         <v>185</v>
       </c>
       <c r="G16" s="36" t="s">
@@ -21617,6 +21614,20 @@
     <row r="1000" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
     <mergeCell ref="E10:E11"/>
@@ -21626,20 +21637,6 @@
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="K10:K11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J12:J14 L12:L14">
     <cfRule type="containsText" dxfId="91" priority="1" operator="containsText" text="FAIL">
@@ -21773,7 +21770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F640670-82B7-42C7-99B2-4336FDCE8589}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
       <selection activeCell="M10" sqref="M10:M16"/>
     </sheetView>
   </sheetViews>
@@ -21787,7 +21784,7 @@
     <col min="6" max="6" width="19.5" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
     <col min="8" max="8" width="20.8984375" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
@@ -21795,14 +21792,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="68" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -21813,14 +21810,14 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="75" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -21831,12 +21828,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -21847,14 +21844,14 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="50" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="31"/>
@@ -21865,10 +21862,10 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -21891,8 +21888,8 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>5</v>
       </c>
@@ -21915,10 +21912,10 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -21941,8 +21938,8 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>5</v>
       </c>
@@ -21979,60 +21976,60 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -22042,18 +22039,18 @@
         <f t="shared" ref="B12:B16" si="0">CONCATENATE($C$2, " - ", A12)</f>
         <v>SQ - 1</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="50" t="s">
         <v>158</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="17"/>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="51" t="s">
         <v>169</v>
       </c>
       <c r="G12" s="35"/>
-      <c r="H12" s="72" t="s">
+      <c r="H12" s="52" t="s">
         <v>170</v>
       </c>
       <c r="I12" s="11">
@@ -22068,7 +22065,7 @@
       <c r="L12" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="73" t="s">
+      <c r="M12" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -22080,22 +22077,22 @@
         <f t="shared" si="0"/>
         <v>SQ - 2</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="50" t="s">
         <v>158</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="71" t="s">
+      <c r="E13" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="F13" s="71" t="s">
+      <c r="F13" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="G13" s="72" t="s">
+      <c r="G13" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="H13" s="72" t="s">
+      <c r="H13" s="52" t="s">
         <v>171</v>
       </c>
       <c r="I13" s="11">
@@ -22110,7 +22107,7 @@
       <c r="L13" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="73" t="s">
+      <c r="M13" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -22122,22 +22119,22 @@
         <f t="shared" si="0"/>
         <v>SQ - 3</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="50" t="s">
         <v>158</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="71" t="s">
+      <c r="E14" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="F14" s="71" t="s">
+      <c r="F14" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="G14" s="72" t="s">
+      <c r="G14" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="H14" s="72" t="s">
+      <c r="H14" s="52" t="s">
         <v>173</v>
       </c>
       <c r="I14" s="11">
@@ -22152,7 +22149,7 @@
       <c r="L14" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="73" t="s">
+      <c r="M14" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -22164,22 +22161,22 @@
         <f t="shared" si="0"/>
         <v>SQ - 4</v>
       </c>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="F15" s="71" t="s">
+      <c r="F15" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G15" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="H15" s="72" t="s">
+      <c r="H15" s="52" t="s">
         <v>177</v>
       </c>
       <c r="I15" s="11">
@@ -22194,7 +22191,7 @@
       <c r="L15" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="73" t="s">
+      <c r="M15" s="53" t="s">
         <v>9</v>
       </c>
     </row>
@@ -22206,19 +22203,19 @@
         <f t="shared" si="0"/>
         <v>SQ - 5</v>
       </c>
-      <c r="C16" s="70" t="s">
+      <c r="C16" s="50" t="s">
         <v>158</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="71" t="s">
+      <c r="E16" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="F16" s="71" t="s">
+      <c r="F16" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="G16" s="72" t="s">
+      <c r="G16" s="52" t="s">
         <v>178</v>
       </c>
       <c r="H16" s="36" t="s">
@@ -22236,12 +22233,26 @@
       <c r="L16" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="73" t="s">
+      <c r="M16" s="53" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
@@ -22251,20 +22262,6 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J12:J14 L12:L14">
     <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="FAIL">
@@ -22371,7 +22368,7 @@
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.69921875" customWidth="1"/>
     <col min="8" max="8" width="21.59765625" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
@@ -22379,14 +22376,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="68" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -22397,14 +22394,14 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="75" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -22415,12 +22412,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -22431,14 +22428,14 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="68" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="31"/>
@@ -22449,10 +22446,10 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -22475,8 +22472,8 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>5</v>
       </c>
@@ -22499,10 +22496,10 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -22525,8 +22522,8 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>5</v>
       </c>
@@ -22563,60 +22560,60 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -22626,18 +22623,18 @@
         <f t="shared" ref="B12:B16" si="0">CONCATENATE($C$2, " - ", A12)</f>
         <v>SQR - 1</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="50" t="s">
         <v>159</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="17"/>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="51" t="s">
         <v>182</v>
       </c>
       <c r="G12" s="35"/>
-      <c r="H12" s="72" t="s">
+      <c r="H12" s="52" t="s">
         <v>170</v>
       </c>
       <c r="I12" s="11">
@@ -22652,7 +22649,7 @@
       <c r="L12" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="73" t="s">
+      <c r="M12" s="53" t="s">
         <v>10</v>
       </c>
     </row>
@@ -22664,22 +22661,22 @@
         <f t="shared" si="0"/>
         <v>SQR - 2</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="50" t="s">
         <v>159</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="71" t="s">
+      <c r="E13" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="F13" s="71" t="s">
+      <c r="F13" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="G13" s="72" t="s">
+      <c r="G13" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="H13" s="72" t="s">
+      <c r="H13" s="52" t="s">
         <v>188</v>
       </c>
       <c r="I13" s="11">
@@ -22694,7 +22691,7 @@
       <c r="L13" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="73" t="s">
+      <c r="M13" s="53" t="s">
         <v>10</v>
       </c>
     </row>
@@ -22706,22 +22703,22 @@
         <f t="shared" si="0"/>
         <v>SQR - 3</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="50" t="s">
         <v>159</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="71" t="s">
+      <c r="E14" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="F14" s="71" t="s">
+      <c r="F14" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="G14" s="72" t="s">
+      <c r="G14" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="H14" s="72" t="s">
+      <c r="H14" s="52" t="s">
         <v>190</v>
       </c>
       <c r="I14" s="11">
@@ -22736,7 +22733,7 @@
       <c r="L14" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="73" t="s">
+      <c r="M14" s="53" t="s">
         <v>10</v>
       </c>
     </row>
@@ -22748,22 +22745,22 @@
         <f t="shared" si="0"/>
         <v>SQR - 4</v>
       </c>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="F15" s="71" t="s">
+      <c r="F15" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G15" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="H15" s="72" t="s">
+      <c r="H15" s="52" t="s">
         <v>177</v>
       </c>
       <c r="I15" s="11">
@@ -22778,7 +22775,7 @@
       <c r="L15" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="73" t="s">
+      <c r="M15" s="53" t="s">
         <v>10</v>
       </c>
     </row>
@@ -22790,19 +22787,19 @@
         <f t="shared" si="0"/>
         <v>SQR - 5</v>
       </c>
-      <c r="C16" s="70" t="s">
+      <c r="C16" s="50" t="s">
         <v>159</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="71" t="s">
+      <c r="E16" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="F16" s="71" t="s">
+      <c r="F16" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="G16" s="72" t="s">
+      <c r="G16" s="52" t="s">
         <v>186</v>
       </c>
       <c r="H16" s="36" t="s">
@@ -22820,12 +22817,26 @@
       <c r="L16" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="73" t="s">
+      <c r="M16" s="53" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
@@ -22835,20 +22846,6 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J12:J14 L12:L14">
     <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="FAIL">
@@ -22942,7 +22939,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B12" sqref="B12:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -22955,7 +22952,7 @@
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.69921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.19921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
@@ -22963,14 +22960,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="68" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="45"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
@@ -22981,14 +22978,14 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="D2" s="45"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -22999,12 +22996,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="59"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -23015,14 +23012,14 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="68" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="31"/>
@@ -23033,10 +23030,10 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="53"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="14" t="s">
         <v>40</v>
       </c>
@@ -23059,8 +23056,8 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10">
         <v>2</v>
       </c>
@@ -23083,10 +23080,10 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="53"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="14" t="s">
         <v>40</v>
       </c>
@@ -23109,8 +23106,8 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="10">
         <v>2</v>
       </c>
@@ -23147,60 +23144,60 @@
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="56" t="s">
+      <c r="I10" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="56" t="s">
+      <c r="J10" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="56" t="s">
+      <c r="K10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="56" t="s">
+      <c r="L10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="63" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="62"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
     </row>
     <row r="12" spans="1:13" ht="100.8" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -23210,22 +23207,22 @@
         <f>CONCATENATE($C$2, " - ", A12)</f>
         <v>BS - 1</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="F12" s="74" t="s">
+      <c r="F12" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="G12" s="75" t="s">
+      <c r="G12" s="55" t="s">
         <v>195</v>
       </c>
-      <c r="H12" s="74" t="s">
+      <c r="H12" s="54" t="s">
         <v>196</v>
       </c>
       <c r="I12" s="11">
@@ -23240,7 +23237,7 @@
       <c r="L12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="73" t="s">
+      <c r="M12" s="53" t="s">
         <v>12</v>
       </c>
     </row>
@@ -23252,22 +23249,22 @@
         <f t="shared" ref="B13" si="0">CONCATENATE($C$2, " - ", A13)</f>
         <v>BS - 2</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="E13" s="70" t="s">
+      <c r="E13" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="F13" s="74" t="s">
+      <c r="F13" s="54" t="s">
         <v>198</v>
       </c>
-      <c r="G13" s="72" t="s">
+      <c r="G13" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="H13" s="74" t="s">
+      <c r="H13" s="54" t="s">
         <v>200</v>
       </c>
       <c r="I13" s="11">
@@ -23282,12 +23279,26 @@
       <c r="L13" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="73" t="s">
+      <c r="M13" s="53" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="K10:K11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
@@ -23297,20 +23308,6 @@
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="J13 L13">
     <cfRule type="containsText" dxfId="47" priority="9" operator="containsText" text="FAIL">

</xml_diff>